<commit_message>
writing for replication, refining done
</commit_message>
<xml_diff>
--- a/0_docs/Replication_Bypass-Refinement.xlsx
+++ b/0_docs/Replication_Bypass-Refinement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wulic\Documents\GitHub\urban_climate_and_who\0_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8930CC95-2251-4C6E-8E54-8BEF9D78ACA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41C88794-2EB7-43CD-90DE-1D36BB360282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
   <si>
     <t>UWG Paper</t>
   </si>
@@ -124,10 +124,6 @@
     Metal Decking;           !- Layer 3</t>
   </si>
   <si>
-    <t xml:space="preserve">
-    HW CONCRETE,             !- Outside Layer</t>
-  </si>
-  <si>
     <t>Construction,
     Steel Frame Res Ext Wall,!- Name
     Wood Siding,             !- Outside Layer
@@ -138,9 +134,6 @@
     <t>VCWGv200-EP➡️</t>
   </si>
   <si>
-    <t>⬅️VCWGv200-EP Name convention</t>
-  </si>
-  <si>
     <t>BaselWall-VCWG-EP</t>
   </si>
   <si>
@@ -154,13 +147,24 @@
 ext-slab,                !- Name
     HW CONCRETE,             !- Outside Layer
     CP02 CARPET PAD;         !- Layer 2</t>
+  </si>
+  <si>
+    <t>0.93 W/m/K, 1.5e6 J/m3/K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    HW CONCRETE, !- Outside Layer</t>
+  </si>
+  <si>
+    <t>⬅️VCWGv200-EP 
+Name convention</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -174,6 +178,14 @@
       <name val="JetBrains Mono"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -183,7 +195,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -191,20 +203,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -486,175 +518,198 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.21875" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" customWidth="1"/>
     <col min="5" max="5" width="37.33203125" customWidth="1"/>
-    <col min="6" max="6" width="39.21875" customWidth="1"/>
-    <col min="7" max="7" width="31" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.44140625" customWidth="1"/>
+    <col min="7" max="7" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="B1" t="s">
+    <row r="1" spans="1:7" ht="28.8">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="67.8" customHeight="1">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" ht="72">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="86.4">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="1" t="s">
+    <row r="5" spans="1:7">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" ht="57.6">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="72">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5">
-        <v>0.15</v>
-      </c>
-      <c r="D5">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="57.6">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" s="1" t="s">
+    <row r="7" spans="1:7" ht="43.2">
+      <c r="A7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" ht="28.8">
+      <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="43.2">
-      <c r="A7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="B8" s="1"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>